<commit_message>
resolved duplicates and moved outpust to clean
</commit_message>
<xml_diff>
--- a/CelticSea/FLBEIA_model/lookup/Metier_lvl4_lookup.xlsx
+++ b/CelticSea/FLBEIA_model/lookup/Metier_lvl4_lookup.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git Repos\wg_WGMIXFISH\CelticSea\FLBEIA_model\lookup\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="c:\git repos\wg_wgmixfish\celticsea\flbeia_model\lookup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{227998F8-6E39-4196-A928-C8B044264893}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E65B8A39-136B-416D-A136-FC2B0523627F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31890" yWindow="1980" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4860" yWindow="1245" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,9 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="58">
   <si>
-    <t>C-Allge</t>
-  </si>
-  <si>
     <t>MIS</t>
   </si>
   <si>
@@ -199,6 +196,9 @@
   </si>
   <si>
     <t>Offshore-Gillnets</t>
+  </si>
+  <si>
+    <t>C-Allgears</t>
   </si>
 </sst>
 </file>
@@ -518,312 +518,315 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>57</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" t="s">
         <v>30</v>
-      </c>
-      <c r="B21" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23" t="s">
         <v>33</v>
-      </c>
-      <c r="B23" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24" t="s">
         <v>35</v>
-      </c>
-      <c r="B24" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B25" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>37</v>
+      </c>
+      <c r="B26" t="s">
         <v>38</v>
-      </c>
-      <c r="B26" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>40</v>
+      </c>
+      <c r="B28" t="s">
         <v>41</v>
-      </c>
-      <c r="B28" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B29" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>43</v>
+      </c>
+      <c r="B30" t="s">
         <v>44</v>
-      </c>
-      <c r="B30" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>45</v>
+      </c>
+      <c r="B31" t="s">
         <v>46</v>
-      </c>
-      <c r="B31" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>47</v>
+      </c>
+      <c r="B32" t="s">
         <v>48</v>
-      </c>
-      <c r="B32" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C33" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C34" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>51</v>
+      </c>
+      <c r="B35" t="s">
+        <v>51</v>
+      </c>
+      <c r="C35" t="s">
         <v>52</v>
-      </c>
-      <c r="B35" t="s">
-        <v>52</v>
-      </c>
-      <c r="C35" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>53</v>
+      </c>
+      <c r="B36" t="s">
         <v>54</v>
-      </c>
-      <c r="B36" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B37" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>